<commit_message>
not sure, but pushing it
</commit_message>
<xml_diff>
--- a/Calibration/deadtime calibration.xlsx
+++ b/Calibration/deadtime calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seanj\Projects\ME121\ME121-Fishtank\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939AED7D-EF3C-43D5-8F41-AC465D0A8F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B7B4F3-52F6-4676-850F-FF72FD39619B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0AFAE9ED-1713-4B0B-888A-98E8047DCA02}"/>
   </bookViews>
@@ -30,10 +30,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>